<commit_message>
Update app.py and questions.xlsx with new questionnaire
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giulia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giulia/Desktop/easyexercise/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6C48505-E407-EF4B-93F2-73EB6B2F667D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDC7CF0-1E84-D042-BC78-2984C03A92E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1260" windowWidth="27640" windowHeight="16460" xr2:uid="{A7799B31-11A1-E849-A7C0-21A84551C890}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>section</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Water used</t>
+  </si>
+  <si>
+    <t>Auxiliar fuel</t>
   </si>
 </sst>
 </file>
@@ -481,7 +484,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -586,9 +589,18 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>